<commit_message>
AutoCommit_25 февраля 2024 г. 16:21:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8560"/>
   </bookViews>
   <sheets>
     <sheet name="Sibirev I. V." sheetId="1" r:id="rId1"/>
@@ -19,41 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>2ИСИП-122: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
   <si>
-    <t>18янв</t>
-  </si>
-  <si>
-    <t>23янв</t>
-  </si>
-  <si>
-    <t>25янв</t>
-  </si>
-  <si>
-    <t>1фев</t>
-  </si>
-  <si>
-    <t>8фев</t>
-  </si>
-  <si>
-    <t>13фев</t>
-  </si>
-  <si>
-    <t>15фев</t>
-  </si>
-  <si>
-    <t>22фев</t>
-  </si>
-  <si>
     <t>Анакина Надежда</t>
   </si>
   <si>
-    <t>Н</t>
-  </si>
-  <si>
     <t>Анджигаев Владислав</t>
   </si>
   <si>
@@ -78,10 +51,6 @@
     <t>Зямилов Никита</t>
   </si>
   <si>
-    <t>5
-                                            5</t>
-  </si>
-  <si>
     <t>Каиров Давид</t>
   </si>
   <si>
@@ -130,10 +99,6 @@
     <t>Федоскова Дарья</t>
   </si>
   <si>
-    <t>5
-                                            УВ</t>
-  </si>
-  <si>
     <t>Федченко Кирилл</t>
   </si>
   <si>
@@ -144,6 +109,21 @@
   </si>
   <si>
     <t>Чжен Денис</t>
+  </si>
+  <si>
+    <t>ДЗ_1</t>
+  </si>
+  <si>
+    <t>ДЗ_2</t>
+  </si>
+  <si>
+    <t>ДЗ_3</t>
+  </si>
+  <si>
+    <t>ДЗ_4</t>
+  </si>
+  <si>
+    <t>ДЗ_5</t>
   </si>
 </sst>
 </file>
@@ -524,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -541,32 +521,24 @@
     </row>
     <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
@@ -584,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -593,142 +565,90 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2">
-        <v>5</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2">
-        <v>5</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2">
-        <v>5</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -738,51 +658,41 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <v>5</v>
-      </c>
+      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -791,28 +701,22 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -822,78 +726,58 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2">
-        <v>5</v>
-      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
-      <c r="K15" s="2">
-        <v>5</v>
-      </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5</v>
-      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -910,7 +794,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -920,16 +804,14 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2">
-        <v>5</v>
-      </c>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -939,85 +821,65 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2">
-        <v>5</v>
-      </c>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>5</v>
-      </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2">
-        <v>5</v>
-      </c>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1034,150 +896,92 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="2">
-        <v>5</v>
-      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
-        <v>5</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="50" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="2">
-        <v>5</v>
-      </c>
-      <c r="H28" s="2">
-        <v>5</v>
-      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="2">
-        <v>5</v>
-      </c>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1187,39 +991,31 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="2">
-        <v>5</v>
-      </c>
+      <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="2">
-        <v>5</v>
-      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
-      <c r="K30" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1229,61 +1025,35 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <v>5</v>
-      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2">
-        <v>5</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="3">
-        <v>1</v>
-      </c>
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="3">
-        <v>1</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1</v>
-      </c>
-      <c r="I33" s="3">
-        <v>1</v>
-      </c>
-      <c r="J33" s="3">
-        <v>1</v>
-      </c>
-      <c r="K33" s="3">
-        <v>1</v>
-      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
AutoCommit_29 февраля 2024 г. 13:47:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -660,9 +660,15 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -796,9 +802,15 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 13:51:37_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -859,10 +859,18 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21" s="2">
+        <v>5</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 11:33:05_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,9 @@
       <c r="E18" s="2">
         <v>5</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 11:45:40_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -683,9 +683,15 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 11:46:40_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -592,9 +592,15 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -757,9 +763,15 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -892,8 +904,12 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 11:49:31_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -845,9 +845,15 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="2">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_4 апреля 2024 г. 12:57:43_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -615,10 +615,18 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -897,7 +905,9 @@
       <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -948,9 +958,15 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -965,10 +981,18 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1033,10 +1057,18 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1050,7 +1082,9 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 12:26:41_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1105,10 +1105,18 @@
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 15:58:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -154,12 +154,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -189,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -199,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,13 +513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -520,12 +529,12 @@
     <col min="3" max="11" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -552,7 +561,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -563,16 +572,22 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -586,17 +601,26 @@
       <c r="M4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -610,21 +634,24 @@
       <c r="M5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4">
         <v>5</v>
       </c>
       <c r="F6" s="2">
@@ -644,21 +671,24 @@
       <c r="M6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
         <v>5</v>
       </c>
       <c r="F7" s="2">
@@ -676,21 +706,24 @@
       <c r="M7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4">
         <v>5</v>
       </c>
       <c r="F8" s="2">
@@ -708,17 +741,26 @@
       <c r="M8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -732,21 +774,24 @@
       <c r="M9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
         <v>5</v>
       </c>
       <c r="F10" s="2"/>
@@ -762,21 +807,24 @@
       <c r="M10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
         <v>5</v>
       </c>
       <c r="F11" s="2"/>
@@ -792,17 +840,26 @@
       <c r="M11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -816,17 +873,26 @@
       <c r="M12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -840,21 +906,24 @@
       <c r="M13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
         <v>5</v>
       </c>
       <c r="F14" s="2">
@@ -872,21 +941,24 @@
       <c r="M14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
         <v>5</v>
       </c>
       <c r="F15" s="2">
@@ -904,17 +976,26 @@
       <c r="M15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -928,19 +1009,26 @@
       <c r="M16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2"/>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
       <c r="F17" s="2">
         <v>5</v>
       </c>
@@ -956,21 +1044,24 @@
       <c r="M17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
         <v>5</v>
       </c>
       <c r="F18" s="2">
@@ -988,21 +1079,24 @@
       <c r="M18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
         <v>5</v>
       </c>
       <c r="F19" s="2"/>
@@ -1018,17 +1112,26 @@
       <c r="M19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1042,21 +1145,24 @@
       <c r="M20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4">
         <v>5</v>
       </c>
       <c r="F21" s="2">
@@ -1076,21 +1182,26 @@
       <c r="M21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1104,17 +1215,26 @@
       <c r="M22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1128,21 +1248,24 @@
       <c r="M23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="C24" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4">
         <v>5</v>
       </c>
       <c r="F24" s="2"/>
@@ -1158,21 +1281,24 @@
       <c r="M24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="C25" s="4">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>5</v>
+      </c>
+      <c r="E25" s="4">
         <v>5</v>
       </c>
       <c r="F25" s="2">
@@ -1190,17 +1316,26 @@
       <c r="M25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1214,17 +1349,26 @@
       <c r="M26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1238,17 +1382,26 @@
       <c r="M27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1262,21 +1415,24 @@
       <c r="M28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
-        <v>5</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="C29" s="4">
+        <v>5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>5</v>
+      </c>
+      <c r="E29" s="4">
         <v>5</v>
       </c>
       <c r="F29" s="2">
@@ -1295,18 +1451,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1321,17 +1481,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
-        <v>5</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="4">
+        <v>5</v>
+      </c>
+      <c r="D31" s="4">
         <v>5</v>
       </c>
       <c r="E31" s="2">
@@ -1353,16 +1513,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 16:15:48_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -154,7 +154,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +164,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -207,6 +213,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -519,7 +528,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -588,7 +597,9 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -621,7 +632,9 @@
       <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -654,10 +667,10 @@
       <c r="E6" s="4">
         <v>5</v>
       </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
         <v>5</v>
       </c>
       <c r="H6" s="2"/>
@@ -691,7 +704,7 @@
       <c r="E7" s="4">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>5</v>
       </c>
       <c r="G7" s="2"/>
@@ -726,7 +739,7 @@
       <c r="E8" s="4">
         <v>5</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <v>5</v>
       </c>
       <c r="G8" s="2"/>
@@ -761,7 +774,9 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -794,7 +809,9 @@
       <c r="E10" s="4">
         <v>5</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -827,7 +844,9 @@
       <c r="E11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -860,7 +879,9 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -893,7 +914,9 @@
       <c r="E13" s="4">
         <v>0</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -926,7 +949,7 @@
       <c r="E14" s="4">
         <v>5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="5">
         <v>5</v>
       </c>
       <c r="G14" s="2"/>
@@ -961,7 +984,7 @@
       <c r="E15" s="4">
         <v>5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="5">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
@@ -996,7 +1019,9 @@
       <c r="E16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1029,7 +1054,7 @@
       <c r="E17" s="4">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="5">
         <v>5</v>
       </c>
       <c r="G17" s="2"/>
@@ -1064,7 +1089,7 @@
       <c r="E18" s="4">
         <v>5</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="5">
         <v>5</v>
       </c>
       <c r="G18" s="2"/>
@@ -1099,7 +1124,9 @@
       <c r="E19" s="4">
         <v>5</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1132,7 +1159,9 @@
       <c r="E20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1165,10 +1194,10 @@
       <c r="E21" s="4">
         <v>5</v>
       </c>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
         <v>5</v>
       </c>
       <c r="H21" s="2"/>
@@ -1202,7 +1231,9 @@
       <c r="E22" s="4">
         <v>0</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1235,7 +1266,9 @@
       <c r="E23" s="4">
         <v>0</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1268,7 +1301,9 @@
       <c r="E24" s="4">
         <v>5</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="5">
+        <v>0</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1301,7 +1336,7 @@
       <c r="E25" s="4">
         <v>5</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="5">
         <v>5</v>
       </c>
       <c r="G25" s="2"/>
@@ -1333,10 +1368,12 @@
       <c r="D26" s="4">
         <v>0</v>
       </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1366,10 +1403,12 @@
       <c r="D27" s="4">
         <v>0</v>
       </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1399,10 +1438,12 @@
       <c r="D28" s="4">
         <v>0</v>
       </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2"/>
+      <c r="E28" s="5">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1432,10 +1473,10 @@
       <c r="D29" s="4">
         <v>5</v>
       </c>
-      <c r="E29" s="4">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="E29" s="5">
+        <v>5</v>
+      </c>
+      <c r="F29" s="5">
         <v>5</v>
       </c>
       <c r="G29" s="2"/>
@@ -1464,10 +1505,12 @@
       <c r="D30" s="4">
         <v>0</v>
       </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2"/>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1494,10 +1537,10 @@
       <c r="D31" s="4">
         <v>5</v>
       </c>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="E31" s="5">
+        <v>5</v>
+      </c>
+      <c r="F31" s="5">
         <v>5</v>
       </c>
       <c r="G31" s="2"/>
@@ -1526,10 +1569,12 @@
       <c r="D32" s="4">
         <v>0</v>
       </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2"/>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:05:41_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -525,10 +525,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1215,7 +1215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1250,33 +1250,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="C23" s="2">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(C23:F23)</f>
+        <v>20</v>
       </c>
       <c r="M23">
         <v>3</v>
@@ -1285,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:06:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -525,10 +525,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1038,33 +1038,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
-        <v>0</v>
+      <c r="C17" s="2">
+        <v>5</v>
       </c>
       <c r="D17" s="4">
         <v>5</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
+      <c r="E17" s="2">
+        <v>5</v>
       </c>
       <c r="F17" s="5">
         <v>5</v>
       </c>
-      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>SUM(C17:F17)</f>
+        <v>20</v>
       </c>
       <c r="M17">
         <v>4</v>
@@ -1073,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_18 апреля 2024 г. 12:24:39_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -528,7 +528,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -623,17 +623,17 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -642,7 +642,7 @@
       <c r="K5" s="2"/>
       <c r="L5">
         <f t="shared" ref="L5:L32" si="0">SUM(C5:G5)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -870,17 +870,17 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -889,7 +889,7 @@
       <c r="K12" s="2"/>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -1430,17 +1430,17 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0</v>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>5</v>
+      </c>
+      <c r="F28" s="2">
+        <v>5</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1449,7 +1449,7 @@
       <c r="K28" s="2"/>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M28">
         <v>3</v>
@@ -1477,14 +1477,16 @@
       <c r="F29" s="5">
         <v>5</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M29">
         <v>5</v>
@@ -1561,26 +1563,28 @@
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5">
-        <v>0</v>
-      </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2"/>
+      <c r="C32" s="2">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M32">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 14:49:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -525,10 +525,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -882,14 +882,16 @@
       <c r="F12" s="2">
         <v>5</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -1055,6 +1057,9 @@
         <v>5</v>
       </c>
       <c r="F17" s="5">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2">
         <v>5</v>
       </c>
       <c r="H17" s="2"/>
@@ -1149,26 +1154,28 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2"/>
+      <c r="C20" s="2">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="M20">
         <v>3</v>
@@ -1266,6 +1273,9 @@
         <v>5</v>
       </c>
       <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
         <v>5</v>
       </c>
       <c r="H23" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_8 мая 2024 г. 9:08:35_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -534,10 +534,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_16 мая 2024 г. 12:21:26_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -534,10 +534,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1033,14 +1033,18 @@
       <c r="F16" s="5">
         <v>2</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="M16">
         <v>3</v>
@@ -1215,8 +1219,12 @@
       <c r="G21" s="5">
         <v>5</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="2">
+        <v>5</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21">
@@ -1499,8 +1507,12 @@
       <c r="G29" s="2">
         <v>5</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="H29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29">

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 13:31:42_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-122: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>ТК</t>
+  </si>
+  <si>
+    <t>ДЗ_6</t>
+  </si>
+  <si>
+    <t>ДЗ_7</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -568,8 +574,12 @@
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
@@ -963,14 +973,20 @@
       <c r="F14" s="5">
         <v>5</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M14">
         <v>3</v>
@@ -1109,14 +1125,20 @@
       <c r="F18" s="5">
         <v>5</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="G18" s="2">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M18">
         <v>5</v>
@@ -1295,8 +1317,12 @@
       <c r="G23" s="2">
         <v>5</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>5</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23">
@@ -1326,17 +1352,23 @@
       <c r="E24" s="4">
         <v>5</v>
       </c>
-      <c r="F24" s="5">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="M24">
         <v>5</v>
@@ -1345,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1364,14 +1396,17 @@
       <c r="F25" s="5">
         <v>5</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>5</v>
+      </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C25:H25)</f>
+        <v>25</v>
       </c>
       <c r="M25">
         <v>5</v>
@@ -1380,7 +1415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 14:14:31_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -540,10 +540,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -828,17 +828,23 @@
       <c r="E10" s="4">
         <v>5</v>
       </c>
-      <c r="F10" s="5">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="M10">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_30 мая 2024 г. 13:48:41_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -540,10 +540,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -610,23 +610,25 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5">
-        <v>2</v>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4">
         <f>SUM(C4:G4)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -869,17 +871,23 @@
       <c r="E11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="5">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="M11">
         <v>5</v>
@@ -932,26 +940,30 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2</v>
-      </c>
-      <c r="F13" s="5">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2">
+        <v>5</v>
+      </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="M13">
         <v>3</v>
@@ -1097,8 +1109,12 @@
       <c r="G17" s="2">
         <v>5</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="2">
+        <v>5</v>
+      </c>
+      <c r="I17" s="2">
+        <v>5</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17">
@@ -1279,20 +1295,26 @@
       <c r="D22" s="4">
         <v>5</v>
       </c>
-      <c r="E22" s="4">
-        <v>2</v>
-      </c>
-      <c r="F22" s="5">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M22">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 10:34:31_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>2ИСИП-122: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>ДЗ_7</t>
+  </si>
+  <si>
+    <t>лаб_1</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -580,7 +583,9 @@
       <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
         <v>35</v>
@@ -1269,7 +1274,9 @@
       <c r="I21" s="2">
         <v>5</v>
       </c>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2">
+        <v>5</v>
+      </c>
       <c r="K21" s="2"/>
       <c r="L21">
         <f t="shared" si="0"/>
@@ -1430,7 +1437,9 @@
       <c r="I25" s="2">
         <v>5</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="2">
+        <v>5</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25">
         <f>SUM(C25:H25)</f>
@@ -1576,7 +1585,9 @@
       <c r="I29" s="2">
         <v>5</v>
       </c>
-      <c r="J29" s="2"/>
+      <c r="J29" s="2">
+        <v>5</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="L29">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 11:01:46_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -543,10 +543,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1120,9 @@
       <c r="I17" s="2">
         <v>5</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
       <c r="K17" s="2"/>
       <c r="L17">
         <f>SUM(C17:F17)</f>
@@ -1358,7 +1360,9 @@
       <c r="I23" s="2">
         <v>5</v>
       </c>
-      <c r="J23" s="2"/>
+      <c r="J23" s="2">
+        <v>5</v>
+      </c>
       <c r="K23" s="2"/>
       <c r="L23">
         <f>SUM(C23:F23)</f>

</xml_diff>

<commit_message>
AutoCommit_31 мая 2024 г. 11:20:43_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -543,10 +543,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1163,7 +1163,9 @@
       <c r="I18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2">
+        <v>5</v>
+      </c>
       <c r="K18" s="2"/>
       <c r="L18">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
AutoCommit_3 июня 2024 г. 8:24:10_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -543,10 +543,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1613,23 +1613,27 @@
       <c r="C30" s="6">
         <v>5</v>
       </c>
-      <c r="D30" s="4">
-        <v>2</v>
-      </c>
-      <c r="E30" s="5">
-        <v>2</v>
-      </c>
-      <c r="F30" s="5">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
+      <c r="H30" s="2">
+        <v>5</v>
+      </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="M30">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_4 июня 2024 г. 13:50:54_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -543,10 +543,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5">
-        <f t="shared" ref="L5:L32" si="0">SUM(C5:G5)</f>
+        <f t="shared" ref="L5:L31" si="0">SUM(C5:G5)</f>
         <v>20</v>
       </c>
       <c r="M5">
@@ -923,13 +923,17 @@
       <c r="G12" s="2">
         <v>5</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>5</v>
+      </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(C12:I12)</f>
+        <v>35</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -1693,13 +1697,17 @@
       <c r="G32" s="2">
         <v>5</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>5</v>
+      </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+      <c r="J32" s="2">
+        <v>5</v>
+      </c>
       <c r="K32" s="2"/>
       <c r="L32">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(C32:H32)</f>
+        <v>30</v>
       </c>
       <c r="M32">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 10:58:27_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -212,11 +212,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +245,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -543,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -699,8 +713,12 @@
       <c r="G6" s="5">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6">
@@ -1441,6 +1459,9 @@
       <c r="F25" s="5">
         <v>5</v>
       </c>
+      <c r="G25" s="7">
+        <v>5</v>
+      </c>
       <c r="H25" s="2">
         <v>5</v>
       </c>
@@ -1453,7 +1474,7 @@
       <c r="K25" s="2"/>
       <c r="L25">
         <f>SUM(C25:H25)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="M25">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 12:25:45_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,9 @@
       <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
AutoCommit_11 июня 2024 г. 21:06:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 8:38:17_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -560,7 +560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -609,11 +609,21 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.25">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -638,16 +648,22 @@
       <c r="F4" s="2">
         <v>5</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
       <c r="H4" s="2">
         <v>5</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4">
         <f>SUM(C4:G4)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -675,14 +691,22 @@
       <c r="F5" s="2">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
       <c r="K5" s="2"/>
       <c r="L5">
-        <f t="shared" ref="L5:L31" si="0">SUM(C5:G5)</f>
-        <v>20</v>
+        <f>SUM(C5:J5)</f>
+        <v>28</v>
       </c>
       <c r="M5">
         <v>3</v>
@@ -719,10 +743,12 @@
       <c r="I6" s="2">
         <v>5</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L6:L31" si="0">SUM(C6:G6)</f>
         <v>25</v>
       </c>
       <c r="M6">
@@ -751,14 +777,22 @@
       <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M7">
         <v>5</v>
@@ -786,14 +820,22 @@
       <c r="F8" s="5">
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M8">
         <v>5</v>
@@ -821,14 +863,22 @@
       <c r="F9" s="5">
         <v>2</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M9">
         <v>3</v>
@@ -865,7 +915,9 @@
       <c r="I10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10">
         <f t="shared" si="0"/>
@@ -949,11 +1001,13 @@
       <c r="I12" s="2">
         <v>5</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12">
-        <f>SUM(C12:I12)</f>
-        <v>35</v>
+        <f>SUM(C12:J12)</f>
+        <v>37</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -984,11 +1038,15 @@
       <c r="G13" s="2">
         <v>5</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
       <c r="I13" s="2">
         <v>5</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13">
         <f t="shared" si="0"/>
@@ -1029,7 +1087,9 @@
       <c r="I14" s="2">
         <v>5</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14">
         <f t="shared" si="0"/>
@@ -1061,14 +1121,22 @@
       <c r="F15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
       <c r="K15" s="2"/>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M15">
         <v>5</v>
@@ -1102,8 +1170,12 @@
       <c r="H16" s="2">
         <v>5</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="I16" s="2">
+        <v>2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
       <c r="K16" s="2"/>
       <c r="L16">
         <f t="shared" si="0"/>
@@ -1221,14 +1293,22 @@
       <c r="F19" s="5">
         <v>2</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M19">
         <v>5</v>
@@ -1259,13 +1339,19 @@
       <c r="G20" s="2">
         <v>5</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2">
+        <v>2</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(C20:J20)</f>
+        <v>31</v>
       </c>
       <c r="M20">
         <v>3</v>
@@ -1345,7 +1431,9 @@
       <c r="I22" s="2">
         <v>5</v>
       </c>
-      <c r="J22" s="2"/>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22">
         <f t="shared" si="0"/>
@@ -1429,7 +1517,9 @@
       <c r="I24" s="2">
         <v>5</v>
       </c>
-      <c r="J24" s="2"/>
+      <c r="J24" s="2">
+        <v>2</v>
+      </c>
       <c r="K24" s="2"/>
       <c r="L24">
         <f t="shared" si="0"/>
@@ -1504,14 +1594,22 @@
       <c r="F26" s="5">
         <v>2</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="G26" s="2">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
       <c r="K26" s="2"/>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M26">
         <v>3</v>
@@ -1539,14 +1637,22 @@
       <c r="F27" s="5">
         <v>2</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="L27">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M27">
         <v>3</v>
@@ -1574,14 +1680,22 @@
       <c r="F28" s="2">
         <v>5</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="G28" s="2">
+        <v>2</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
       <c r="K28" s="2"/>
       <c r="L28">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C28:J28)</f>
+        <v>28</v>
       </c>
       <c r="M28">
         <v>3</v>
@@ -1655,8 +1769,12 @@
       <c r="H30" s="2">
         <v>5</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="I30" s="2">
+        <v>2</v>
+      </c>
+      <c r="J30" s="2">
+        <v>2</v>
+      </c>
       <c r="K30" s="2"/>
       <c r="L30">
         <f t="shared" si="0"/>
@@ -1685,14 +1803,22 @@
       <c r="F31" s="5">
         <v>5</v>
       </c>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="G31" s="2">
+        <v>2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
       <c r="K31" s="2"/>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M31">
         <v>5</v>
@@ -1723,7 +1849,9 @@
       <c r="H32" s="2">
         <v>5</v>
       </c>
-      <c r="I32" s="2"/>
+      <c r="I32" s="2">
+        <v>2</v>
+      </c>
       <c r="J32" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:00:39_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -916,7 +916,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 11:40:41_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6">
@@ -1122,21 +1122,21 @@
         <v>5</v>
       </c>
       <c r="G15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J15" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="M15">
         <v>5</v>
@@ -1804,21 +1804,21 @@
         <v>5</v>
       </c>
       <c r="G31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J31" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="M31">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 8:44:59_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 10:11:58_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1002,12 +1002,12 @@
         <v>5</v>
       </c>
       <c r="J12" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12">
         <f>SUM(C12:J12)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -1850,7 +1850,7 @@
         <v>5</v>
       </c>
       <c r="I32" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J32" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 10:39:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -560,7 +560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <f>SUM(C8:G8)</f>
         <v>22</v>
       </c>
       <c r="M8">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 13:56:12_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1681,21 +1681,21 @@
         <v>5</v>
       </c>
       <c r="G28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J28" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28">
         <f>SUM(C28:J28)</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M28">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 14:05:41_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -692,21 +692,21 @@
         <v>5</v>
       </c>
       <c r="G5" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I5" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J5" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5">
         <f>SUM(C5:J5)</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M5">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 18:27:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -624,9 +624,15 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 11:40:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-122_ТерВер.xlsx
+++ b/_2ИСИП-122_ТерВер.xlsx
@@ -554,10 +554,10 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>